<commit_message>
Lexer: complete lab1 requirement
</commit_message>
<xml_diff>
--- a/C-1/doc/lexcimal_code.xlsx
+++ b/C-1/doc/lexcimal_code.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GithubRepo\C-1\C-1\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1584A6DD-9B18-4928-A389-30362BA3367B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7ECB69-167A-4C4C-A455-3C69146BB3A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10740" yWindow="330" windowWidth="8265" windowHeight="10110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="121">
   <si>
     <t>sizeof</t>
   </si>
@@ -486,6 +486,14 @@
   </si>
   <si>
     <t>EXP=[eE][+-]?[1-9][0-9]*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OP_ASSIGN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>REL_OP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -532,7 +540,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,6 +559,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -564,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -574,6 +594,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -856,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1057,32 +1080,35 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="11" t="s">
         <v>47</v>
       </c>
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="11" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1136,52 +1162,55 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="A35" s="10" t="s">
         <v>58</v>
       </c>
+      <c r="C35" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="A36" s="10" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="A38" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="A39" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="A40" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="A41" s="10" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="A42" s="10" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="A43" s="10" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="A44" s="10" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1271,45 +1300,45 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="A57" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="A58" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="A59" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="A60" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="A61" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="A62" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="A63" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="A64" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D64" s="1"/>

</xml_diff>